<commit_message>
change template name for one of the kpis
</commit_message>
<xml_diff>
--- a/Projects/CCBZA/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,6 +26,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$S$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$114</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$114</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$S$114</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -498,7 +499,7 @@
     <t xml:space="preserve">SSD IC, SSD FC, Twist and Stills greater than 50% of Competitor of category</t>
   </si>
   <si>
-    <t xml:space="preserve">CCBSA Cooler, DOC Coolers</t>
+    <t xml:space="preserve">DOC Cooler</t>
   </si>
   <si>
     <t xml:space="preserve">Min 4 x Cooler Doors</t>
@@ -1126,19 +1127,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.7627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7953488372093"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,15 +1553,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,23 +1622,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.8697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="144.841860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="83.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.0837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="149.274418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="86.1441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5328,16 +5329,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.506976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6236,31 +6237,31 @@
   </sheetPr>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.0046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6459,17 +6460,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7100,34 +7101,34 @@
   </sheetPr>
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D83" activeCellId="0" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.1302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="149.395348837209"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.7116279069767"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="153.948837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10653,7 +10654,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
         <v>33</v>
       </c>
@@ -10697,7 +10698,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
         <v>33</v>
       </c>

</xml_diff>